<commit_message>
erro a calcular fwhm
Olá
</commit_message>
<xml_diff>
--- a/beta/Beta.xlsx
+++ b/beta/Beta.xlsx
@@ -323,38 +323,38 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -710,7 +710,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="18">
+      <c r="A2" s="17">
         <v>0.1</v>
       </c>
       <c r="B2" s="1">
@@ -719,57 +719,57 @@
       <c r="C2" s="1">
         <v>38</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="18">
         <f>SQRT((POWER((B2-E2),2)*C2+POWER((B3-E2),2)*C3+POWER((B4-E2),2)*C4+POWER((B5-E2),2)*C5)/SUM(C2:C5))</f>
         <v>0.64360105495582876</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="18">
         <f>(B2*C2+B3*C3+B4*C4+B5*C5)/(SUM(C2:C5))</f>
         <v>21.471674876847292</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="18">
         <f>D2/SQRT(SUM(C2:C5))</f>
         <v>2.2585969257828763E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="18"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="1">
         <v>21</v>
       </c>
       <c r="C3" s="1">
         <v>382</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="18"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1">
         <v>22</v>
       </c>
       <c r="C4" s="1">
         <v>363</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="18"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1">
         <v>23</v>
       </c>
       <c r="C5" s="1">
         <v>29</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="18">
+      <c r="A6" s="17">
         <v>0.3</v>
       </c>
       <c r="B6" s="1">
@@ -778,42 +778,42 @@
       <c r="C6" s="1">
         <v>121</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="18">
         <f>SQRT((POWER((B6-E6),2)*C6+POWER((B7-E6),2)*C7+POWER((B8-E6),2)*C8)/SUM(C6:C8))</f>
         <v>0.61469116016393355</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <f>(B6*C6+B7*C7+B8*C8)/(SUM(C6:C8))</f>
         <v>65.083437110834367</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="18">
         <f>D6/SQRT(SUM(C6:C8))</f>
         <v>2.1691979981008913E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="18"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1">
         <v>65</v>
       </c>
       <c r="C7" s="1">
         <v>494</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="19"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="18"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1">
         <v>66</v>
       </c>
       <c r="C8" s="1">
         <v>188</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="19"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="20">
@@ -825,15 +825,15 @@
       <c r="C9" s="1">
         <v>132</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <f>SQRT((POWER((B9-E9),2)*C9+POWER((B10-E9),2)*C10+POWER(B11-E9,2)*C11)/SUM(C9:C11))</f>
         <v>0.62995483661343943</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="18">
         <f>(B9*C9+B10*C10+B11*C11)/(SUM(C9:C11))</f>
         <v>111.07347447073475</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="18">
         <f>D9/SQRT(SUM(C9:C11))</f>
         <v>2.2230623425777141E-2</v>
       </c>
@@ -846,9 +846,9 @@
       <c r="C10" s="1">
         <v>480</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="20"/>
@@ -858,12 +858,12 @@
       <c r="C11" s="1">
         <v>191</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="18">
+      <c r="A12" s="17">
         <v>0.7</v>
       </c>
       <c r="B12" s="1">
@@ -872,45 +872,45 @@
       <c r="C12" s="1">
         <v>187</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <f>SQRT((POWER((B12-E12),2)*C12+POWER((B13-E12),2)*C13+POWER(B14-E12,2)*C14)/SUM(C12:C14))</f>
         <v>0.63702540715324474</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="18">
         <f>(B12*C12+B13*C13+B14*C14)/(SUM(C12:C14))</f>
         <v>152.94117647058823</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="18">
         <f>D12/SQRT(SUM(C12:C15))</f>
         <v>2.0832958497102285E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="18"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1">
         <v>153</v>
       </c>
       <c r="C13" s="1">
         <v>472</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="18"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="1">
         <v>154</v>
       </c>
       <c r="C14" s="1">
         <v>140</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="18">
+      <c r="A15" s="17">
         <v>0.9</v>
       </c>
       <c r="B15" s="1">
@@ -919,45 +919,45 @@
       <c r="C15" s="1">
         <v>136</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="18">
         <f>SQRT((POWER((B15-E15),2)*C15+POWER((B16-E15),2)*C16+POWER(B17-E15,2)*C17)/SUM(C15:C17))</f>
         <v>0.59945631472517569</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="18">
         <f>(B15*C15+B16*C16+B17*C17)/(SUM(C15:C17))</f>
         <v>198.00520833333334</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="18">
         <f>D15/SQRT(SUM(C15:C17))</f>
         <v>2.1631016542125077E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="18"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="1">
         <v>198</v>
       </c>
       <c r="C16" s="1">
         <v>492</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="18"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="1">
         <v>199</v>
       </c>
       <c r="C17" s="1">
         <v>140</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="18">
+      <c r="A18" s="17">
         <v>1.1000000000000001</v>
       </c>
       <c r="B18" s="1">
@@ -966,55 +966,55 @@
       <c r="C18" s="1">
         <v>154</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="18">
         <f>SQRT((POWER((B18-E18),2)*C18+POWER((B19-E18),2)*C19+POWER(B20-E18,2)*C20)/SUM(C18:C20))</f>
         <v>0.62956592705577619</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="18">
         <f>(B18*C18+B19*C19+B20*C20)/(SUM(C18:C20))</f>
         <v>242.01246882793018</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="18">
         <f>D18/SQRT(SUM(C18:C20))</f>
         <v>2.2230745725194487E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="18"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="1">
         <v>242</v>
       </c>
       <c r="C19" s="1">
         <v>484</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="18"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="1">
         <v>243</v>
       </c>
       <c r="C20" s="1">
         <v>164</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="H22" s="17" t="s">
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="H22" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
@@ -1077,12 +1077,12 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
@@ -1114,22 +1114,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="H22:K22"/>
     <mergeCell ref="A26:D26"/>
@@ -1141,6 +1125,22 @@
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="F18:F20"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1459,12 +1459,12 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
@@ -1535,38 +1535,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="P1" s="17" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="P1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="W1" s="17" t="s">
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="W1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -1643,7 +1643,7 @@
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="1">
@@ -1652,34 +1652,34 @@
       <c r="C3" s="1">
         <v>893</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="23">
         <v>3739.75</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="23">
         <v>293.38299999999998</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="23">
         <v>-28.5169</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="23">
         <v>2.7662</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="24">
         <v>104.224</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="24">
         <v>1.0400899999999999E-2</v>
       </c>
-      <c r="J3" s="23">
+      <c r="J3" s="24">
         <v>0.72657300000000002</v>
       </c>
-      <c r="K3" s="23">
+      <c r="K3" s="24">
         <v>9.1839399999999998E-3</v>
       </c>
-      <c r="L3" s="22">
+      <c r="L3" s="25">
         <v>8637.7000000000007</v>
       </c>
-      <c r="M3" s="22">
+      <c r="M3" s="25">
         <v>118.205</v>
       </c>
       <c r="P3" s="1">
@@ -1723,67 +1723,67 @@
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A4" s="17"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1">
         <v>101</v>
       </c>
       <c r="C4" s="1">
         <v>835</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A5" s="17"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1">
         <v>102</v>
       </c>
       <c r="C5" s="1">
         <v>959</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="P5" s="17" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="P5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="1">
         <v>103</v>
       </c>
       <c r="C6" s="1">
         <v>1971</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
       <c r="P6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1798,23 +1798,23 @@
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A7" s="17"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="1">
         <v>104</v>
       </c>
       <c r="C7" s="1">
         <v>5228</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
       <c r="P7" s="1">
         <v>4.5357000000000003</v>
       </c>
@@ -1829,42 +1829,42 @@
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="1">
         <v>105</v>
       </c>
       <c r="C8" s="1">
         <v>3514</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1">
         <v>106</v>
       </c>
       <c r="C9" s="1">
         <v>872</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
       <c r="P9" t="s">
         <v>35</v>
       </c>
@@ -1900,23 +1900,23 @@
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="1">
         <v>107</v>
       </c>
       <c r="C10" s="1">
         <v>650</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
       <c r="P10">
         <v>104.224</v>
       </c>
@@ -1961,23 +1961,23 @@
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="1">
         <v>108</v>
       </c>
       <c r="C11" s="1">
         <v>633</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
       <c r="P11">
         <v>116.05800000000001</v>
       </c>
@@ -2022,23 +2022,23 @@
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="1">
         <v>109</v>
       </c>
       <c r="C12" s="1">
         <v>667</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
       <c r="P12">
         <v>211.346</v>
       </c>
@@ -2083,23 +2083,23 @@
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A13" s="17"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="1">
         <v>110</v>
       </c>
       <c r="C13" s="1">
         <v>644</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
       <c r="P13">
         <v>227.161</v>
       </c>
@@ -2138,7 +2138,7 @@
       <c r="Z13" s="26"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="1">
@@ -2147,74 +2147,74 @@
       <c r="C14" s="1">
         <v>574</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="23">
         <v>598.72400000000005</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="23">
         <v>9.7213499999999993</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="24">
         <v>116.05800000000001</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="24">
         <v>3.8230399999999998E-2</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="24">
         <v>0.79620800000000003</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="24">
         <v>4.6525400000000001E-2</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="25">
         <v>1597.41</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="25">
         <v>80.297200000000004</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A15" s="17"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="1">
         <v>112</v>
       </c>
       <c r="C15" s="1">
         <v>599</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A16" s="17"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="1">
         <v>113</v>
       </c>
       <c r="C16" s="1">
         <v>594</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
       <c r="P16" t="s">
         <v>11</v>
       </c>
@@ -2241,23 +2241,23 @@
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A17" s="17"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="1">
         <v>114</v>
       </c>
       <c r="C17" s="1">
         <v>596</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
       <c r="P17" s="5">
         <f>90524/1000</f>
         <v>90.524000000000001</v>
@@ -2290,23 +2290,23 @@
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A18" s="17"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="1">
         <v>115</v>
       </c>
       <c r="C18" s="1">
         <v>922</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
       <c r="T18">
         <v>2</v>
       </c>
@@ -2327,23 +2327,23 @@
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A19" s="17"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="1">
         <v>116</v>
       </c>
       <c r="C19" s="1">
         <v>1427</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
       <c r="Q19">
         <v>16388</v>
       </c>
@@ -2352,23 +2352,23 @@
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A20" s="17"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="1">
         <v>117</v>
       </c>
       <c r="C20" s="1">
         <v>950</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
       <c r="Q20">
         <v>15711</v>
       </c>
@@ -2377,23 +2377,23 @@
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A21" s="17"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="1">
         <v>118</v>
       </c>
       <c r="C21" s="1">
         <v>765</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
       <c r="Q21">
         <v>13419</v>
       </c>
@@ -2402,70 +2402,70 @@
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A22" s="17"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="1">
         <v>119</v>
       </c>
       <c r="C22" s="1">
         <v>717</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
       <c r="R22">
         <v>2688</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A23" s="17"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="1">
         <v>120</v>
       </c>
       <c r="C23" s="1">
         <v>568</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
       <c r="R23">
         <v>2580</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A24" s="17"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="1">
         <v>121</v>
       </c>
       <c r="C24" s="1">
         <v>528</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="21" t="s">
         <v>50</v>
       </c>
       <c r="B25" s="1">
@@ -2474,229 +2474,229 @@
       <c r="C25" s="1">
         <v>141</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="23">
         <v>2627.17</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="23">
         <v>-12.102399999999999</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="23">
         <v>176.779</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="23">
         <v>0.83528199999999997</v>
       </c>
-      <c r="H25" s="23">
+      <c r="H25" s="24">
         <v>211.346</v>
       </c>
-      <c r="I25" s="23">
+      <c r="I25" s="24">
         <v>1.8996800000000001E-2</v>
       </c>
-      <c r="J25" s="23">
+      <c r="J25" s="24">
         <v>0.77722000000000002</v>
       </c>
-      <c r="K25" s="23">
+      <c r="K25" s="24">
         <v>1.5429200000000001E-2</v>
       </c>
-      <c r="L25" s="22">
+      <c r="L25" s="25">
         <v>2359.21</v>
       </c>
-      <c r="M25" s="22">
+      <c r="M25" s="25">
         <v>53.866999999999997</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A26" s="17"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="1">
         <v>206</v>
       </c>
       <c r="C26" s="1">
         <v>131</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="1">
         <v>207</v>
       </c>
       <c r="C27" s="1">
         <v>121</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A28" s="17"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="1">
         <v>208</v>
       </c>
       <c r="C28" s="1">
         <v>105</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A29" s="17"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="1">
         <v>209</v>
       </c>
       <c r="C29" s="1">
         <v>139</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A30" s="17"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="1">
         <v>210</v>
       </c>
       <c r="C30" s="1">
         <v>372</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A31" s="17"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="1">
         <v>211</v>
       </c>
       <c r="C31" s="1">
         <v>1120</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A32" s="17"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="1">
         <v>212</v>
       </c>
       <c r="C32" s="1">
         <v>972</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="17"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="1">
         <v>213</v>
       </c>
       <c r="C33" s="1">
         <v>154</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="17"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="1">
         <v>214</v>
       </c>
       <c r="C34" s="1">
         <v>34</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="17"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="1">
         <v>215</v>
       </c>
       <c r="C35" s="1">
         <v>31</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
     </row>
     <row r="36" spans="1:13" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="27" t="s">
         <v>51</v>
       </c>
       <c r="B36" s="1">
@@ -2705,294 +2705,278 @@
       <c r="C36" s="1">
         <v>33</v>
       </c>
-      <c r="D36" s="25">
+      <c r="D36" s="23">
         <v>29.043600000000001</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="23">
         <v>2.0008699999999999</v>
       </c>
-      <c r="F36" s="25" t="s">
+      <c r="F36" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G36" s="25" t="s">
+      <c r="G36" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H36" s="23">
+      <c r="H36" s="24">
         <v>227.161</v>
       </c>
-      <c r="I36" s="23">
+      <c r="I36" s="24">
         <v>5.6705699999999998E-2</v>
       </c>
-      <c r="J36" s="23">
+      <c r="J36" s="24">
         <v>0.81362599999999996</v>
       </c>
-      <c r="K36" s="23">
+      <c r="K36" s="24">
         <v>5.8854299999999998E-2</v>
       </c>
-      <c r="L36" s="22">
+      <c r="L36" s="25">
         <v>357.74700000000001</v>
       </c>
-      <c r="M36" s="22">
+      <c r="M36" s="25">
         <v>24.202999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="24"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="1">
         <v>221</v>
       </c>
       <c r="C37" s="1">
         <v>28</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="24"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="1">
         <v>222</v>
       </c>
       <c r="C38" s="1">
         <v>24</v>
       </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="25"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="24"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="1">
         <v>223</v>
       </c>
       <c r="C39" s="1">
         <v>36</v>
       </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="24"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="1">
         <v>224</v>
       </c>
       <c r="C40" s="1">
         <v>24</v>
       </c>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="23"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="24"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="1">
         <v>225</v>
       </c>
       <c r="C41" s="1">
         <v>33</v>
       </c>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="24"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="1">
         <v>226</v>
       </c>
       <c r="C42" s="1">
         <v>91</v>
       </c>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="24"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="1">
         <v>227</v>
       </c>
       <c r="C43" s="1">
         <v>206</v>
       </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="24"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="1">
         <v>228</v>
       </c>
       <c r="C44" s="1">
         <v>127</v>
       </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="24"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="1">
         <v>229</v>
       </c>
       <c r="C45" s="1">
         <v>46</v>
       </c>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="25"/>
+      <c r="M45" s="25"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="24"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="1">
         <v>300</v>
       </c>
       <c r="C46" s="1">
         <v>73</v>
       </c>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="25"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="24"/>
+      <c r="A47" s="27"/>
       <c r="B47" s="1">
         <v>301</v>
       </c>
       <c r="C47" s="1">
         <v>20</v>
       </c>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="22"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="25"/>
+      <c r="M47" s="25"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A48" s="24"/>
+      <c r="A48" s="27"/>
       <c r="B48" s="1">
         <v>302</v>
       </c>
       <c r="C48" s="1">
         <v>0</v>
       </c>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="24"/>
+      <c r="L48" s="25"/>
+      <c r="M48" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="W1:AB1"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="D3:D13"/>
-    <mergeCell ref="E3:E13"/>
-    <mergeCell ref="F3:F13"/>
-    <mergeCell ref="G3:G13"/>
-    <mergeCell ref="H3:H13"/>
-    <mergeCell ref="I3:I13"/>
-    <mergeCell ref="J3:J13"/>
-    <mergeCell ref="K3:K13"/>
-    <mergeCell ref="L3:L13"/>
-    <mergeCell ref="M3:M13"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="Y12:Y13"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="L14:L24"/>
-    <mergeCell ref="A14:A24"/>
-    <mergeCell ref="D14:D24"/>
-    <mergeCell ref="E14:E24"/>
-    <mergeCell ref="F14:F24"/>
-    <mergeCell ref="G14:G24"/>
+    <mergeCell ref="M36:M48"/>
+    <mergeCell ref="H36:H48"/>
+    <mergeCell ref="I36:I48"/>
+    <mergeCell ref="J36:J48"/>
+    <mergeCell ref="K36:K48"/>
+    <mergeCell ref="L36:L48"/>
+    <mergeCell ref="A36:A48"/>
+    <mergeCell ref="D36:D48"/>
+    <mergeCell ref="E36:E48"/>
+    <mergeCell ref="F36:F48"/>
+    <mergeCell ref="G36:G48"/>
     <mergeCell ref="M14:M24"/>
     <mergeCell ref="A25:A35"/>
     <mergeCell ref="D25:D35"/>
@@ -3009,17 +2993,33 @@
     <mergeCell ref="I14:I24"/>
     <mergeCell ref="J14:J24"/>
     <mergeCell ref="K14:K24"/>
-    <mergeCell ref="A36:A48"/>
-    <mergeCell ref="D36:D48"/>
-    <mergeCell ref="E36:E48"/>
-    <mergeCell ref="F36:F48"/>
-    <mergeCell ref="G36:G48"/>
-    <mergeCell ref="M36:M48"/>
-    <mergeCell ref="H36:H48"/>
-    <mergeCell ref="I36:I48"/>
-    <mergeCell ref="J36:J48"/>
-    <mergeCell ref="K36:K48"/>
-    <mergeCell ref="L36:L48"/>
+    <mergeCell ref="L14:L24"/>
+    <mergeCell ref="A14:A24"/>
+    <mergeCell ref="D14:D24"/>
+    <mergeCell ref="E14:E24"/>
+    <mergeCell ref="F14:F24"/>
+    <mergeCell ref="G14:G24"/>
+    <mergeCell ref="M3:M13"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="Y12:Y13"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="H3:H13"/>
+    <mergeCell ref="I3:I13"/>
+    <mergeCell ref="J3:J13"/>
+    <mergeCell ref="K3:K13"/>
+    <mergeCell ref="L3:L13"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="D3:D13"/>
+    <mergeCell ref="E3:E13"/>
+    <mergeCell ref="F3:F13"/>
+    <mergeCell ref="G3:G13"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="W1:AB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3076,7 +3076,7 @@
   <dimension ref="B2:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="B2:K7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3173,29 +3173,29 @@
       <c r="E4" s="7">
         <v>0.22675744430732078</v>
       </c>
-      <c r="F4" s="14">
-        <f t="shared" ref="F4:G7" si="0">E10/2.355</f>
-        <v>0.30852356687898091</v>
-      </c>
-      <c r="G4" s="14">
-        <f t="shared" si="0"/>
-        <v>3.8997622080679407E-3</v>
+      <c r="F4" s="13">
+        <f>E10*2.355</f>
+        <v>1.7110794149999999</v>
+      </c>
+      <c r="G4" s="13">
+        <f>F10*2.355</f>
+        <v>2.16281787E-2</v>
       </c>
       <c r="H4" s="10">
         <f>F4*Bismuto!Y$3</f>
-        <v>1.3955089505258234</v>
+        <v>7.7395275273399786</v>
       </c>
       <c r="I4" s="10">
         <f>SQRT((F4*Bismuto!Z$3)^2+(Bismuto!Y$3*G4)^2)</f>
-        <v>1.7650155202980685E-2</v>
-      </c>
-      <c r="J4" s="15">
+        <v>9.7888202009610958E-2</v>
+      </c>
+      <c r="J4" s="10">
         <f>H4/D4 *100</f>
-        <v>0.29787339808324276</v>
-      </c>
-      <c r="K4" s="15">
+        <v>1.6520133126046161</v>
+      </c>
+      <c r="K4" s="10">
         <f>SQRT((I4/D4)^2+(H4*E4/(D4)^2)^2)*100</f>
-        <v>3.770208790489876E-3</v>
+        <v>2.0909672207276617E-2</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -3210,28 +3210,28 @@
         <v>0.29781798423779776</v>
       </c>
       <c r="F5" s="13">
-        <f t="shared" si="0"/>
-        <v>0.33809256900212314</v>
+        <f t="shared" ref="F5:F7" si="0">E11*2.355</f>
+        <v>1.8750698400000001</v>
       </c>
       <c r="G5" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F4:G7" si="1">F11/2.355</f>
         <v>1.9756008492569001E-2</v>
       </c>
       <c r="H5" s="7">
         <f>F5*Bismuto!Y$3</f>
-        <v>1.5292549963737501</v>
+        <v>8.4812864412637268</v>
       </c>
       <c r="I5" s="10">
         <f>SQRT((F5*Bismuto!Z$3)^2+(Bismuto!Y$3*G5)^2)</f>
-        <v>8.9362630936500737E-2</v>
+        <v>8.9438889119812293E-2</v>
       </c>
       <c r="J5" s="10">
         <f>H5/D5 *100</f>
-        <v>0.29329238114729456</v>
+        <v>1.6266068781524243</v>
       </c>
       <c r="K5" s="10">
         <f>SQRT((I5/D5)^2+(H5*E5/(D5)^2)^2)*100</f>
-        <v>1.7139476990633312E-2</v>
+        <v>1.7178426454003189E-2</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
@@ -3247,27 +3247,27 @@
       </c>
       <c r="F6" s="14">
         <f t="shared" si="0"/>
-        <v>0.33002972399150743</v>
+        <v>1.8303531</v>
       </c>
       <c r="G6" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.5516772823779193E-3</v>
       </c>
       <c r="H6" s="10">
         <f>F6*Bismuto!Y$3</f>
-        <v>1.4927852624962397</v>
+        <v>8.279024385435708</v>
       </c>
       <c r="I6" s="10">
         <f>SQRT((F6*Bismuto!Z$3)^2+(Bismuto!Y$3*G6)^2)</f>
-        <v>2.964180925207522E-2</v>
+        <v>2.9860163256065064E-2</v>
       </c>
       <c r="J6" s="15">
-        <f t="shared" ref="J6:J7" si="1">H6/D6 *100</f>
-        <v>0.15754704865710656</v>
+        <f t="shared" ref="J6:J7" si="2">H6/D6 *100</f>
+        <v>0.87375987052852944</v>
       </c>
       <c r="K6" s="15">
-        <f t="shared" ref="K6:K7" si="2">SQRT((I6/D6)^2+(H6*E6/(D6)^2)^2)*100</f>
-        <v>3.1292012556446364E-3</v>
+        <f t="shared" ref="K6:K7" si="3">SQRT((I6/D6)^2+(H6*E6/(D6)^2)^2)*100</f>
+        <v>3.176797382246254E-3</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -3283,27 +3283,27 @@
       </c>
       <c r="F7" s="13">
         <f t="shared" si="0"/>
-        <v>0.34548874734607216</v>
+        <v>1.9160892299999999</v>
       </c>
       <c r="G7" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.4991210191082802E-2</v>
       </c>
       <c r="H7" s="7">
         <f>F7*Bismuto!Y$3</f>
-        <v>1.5627092740585231</v>
-      </c>
-      <c r="I7" s="10">
+        <v>8.6668247016604205</v>
+      </c>
+      <c r="I7" s="7">
         <f>SQRT((F7*Bismuto!Z$3)^2+(Bismuto!Y$3*G7)^2)</f>
-        <v>0.11304196561121307</v>
+        <v>0.11310492544932578</v>
       </c>
       <c r="J7" s="10">
-        <f t="shared" si="1"/>
-        <v>0.15347184736146988</v>
+        <f t="shared" si="2"/>
+        <v>0.85115870226289592</v>
       </c>
       <c r="K7" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1101998521544735E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.1116490849602118E-2</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">

</xml_diff>